<commit_message>
Add cable; update docs
</commit_message>
<xml_diff>
--- a/Docs/AT-SF1P.CBL01.xlsx
+++ b/Docs/AT-SF1P.CBL01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\SF-1P\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0D7D5D-0FD0-4B2C-BE4C-7B05750B0CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE8608B-4AD1-4642-A6B9-5C23B0012929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1455" windowWidth="20895" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="540" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
-    <t>NBZ-9P+TCTC-9</t>
-  </si>
-  <si>
     <t>Catalog number</t>
   </si>
   <si>
@@ -52,10 +49,6 @@
   </si>
   <si>
     <t>Quantity</t>
-  </si>
-  <si>
-    <t>DB9 MALE
-NBZ-9P+TCTC-9</t>
   </si>
   <si>
     <t>Cable type:</t>
@@ -106,6 +99,13 @@
       </rPr>
       <t xml:space="preserve"> to the cable</t>
     </r>
+  </si>
+  <si>
+    <t>DB9 MALE
+DN-9P+TCTC-9</t>
+  </si>
+  <si>
+    <t>DN-9P+TCTC-9</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -665,13 +665,13 @@
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="9"/>
     </row>
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -689,7 +689,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="10"/>
     </row>
@@ -701,7 +701,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="6">
         <v>120</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -717,10 +717,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="18"/>
     </row>
@@ -730,18 +730,18 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3">
         <f>C10</f>
@@ -769,7 +769,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>